<commit_message>
date time function changes
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2020\MarsQA_2\marsframework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC173C-C66E-4A24-91A0-F397DF1F8E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA133BBA-3B8F-44F4-B027-73446E8E8DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Url</t>
   </si>
@@ -207,12 +207,6 @@
     <t>Project</t>
   </si>
   <si>
-    <t>Technical</t>
-  </si>
-  <si>
-    <t>Test Anyalst</t>
-  </si>
-  <si>
     <t>Testing123</t>
   </si>
   <si>
@@ -226,6 +220,18 @@
   </si>
   <si>
     <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Select day</t>
+  </si>
+  <si>
+    <t>Writing &amp; Translation</t>
+  </si>
+  <si>
+    <t>Creative Writing</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +841,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:K11"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,10 +888,10 @@
         <v>40</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
@@ -917,16 +923,14 @@
         <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="3">
-        <v>44122</v>
-      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="3">
-        <v>44132</v>
+        <v>44193</v>
       </c>
       <c r="J2" s="7">
         <v>0.75</v>
@@ -949,7 +953,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J3" s="7">
-        <v>0.79166666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="K3" s="7">
         <v>0.875</v>
@@ -971,10 +975,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937377EC-4336-4F35-9A85-D326635D076E}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,15 +988,15 @@
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="7" max="8" width="19.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1014,35 +1018,38 @@
       <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1050,13 +1057,13 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -1064,52 +1071,56 @@
       <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="3">
-        <v>43567</v>
+      <c r="H2" t="s">
+        <v>65</v>
       </c>
       <c r="I2" s="3">
-        <v>43597</v>
-      </c>
-      <c r="J2" t="s">
+        <v>44123</v>
+      </c>
+      <c r="J2" s="3">
+        <v>44129</v>
+      </c>
+      <c r="K2" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>0.75</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <v>0.83333333333333337</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>45</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>46</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="K3" s="7">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L3" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>0.875</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="K4" s="7">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L4" s="7">
         <v>0.875</v>
       </c>
-      <c r="L4" s="7">
+      <c r="M4" s="7">
         <v>0.95833333333333337</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>